<commit_message>
update 6way conn BOM
</commit_message>
<xml_diff>
--- a/MUV Kit/Hardware/BOM_sensors_kit.xlsx
+++ b/MUV Kit/Hardware/BOM_sensors_kit.xlsx
@@ -312,9 +312,6 @@
     <t>Gas pcb</t>
   </si>
   <si>
-    <t>https://nl.farnell.com/harwin/m22-7130642/socket-vertical-1row-6way/dp/1109731</t>
-  </si>
-  <si>
     <t>M22-7130642 - Board-To-Board Connector, Vertical, 2 mm, 6 Contacts, Receptacle, M22 Series, Through Hole, 1 Rows</t>
   </si>
   <si>
@@ -463,6 +460,9 @@
   </si>
   <si>
     <t>https://nl.farnell.com/webapp/wcs/stores/servlet/ProductDisplay?urlRequestType=Base&amp;catalogId=10001&amp;langId=31&amp;storeId=10168&amp;partNumber=2675010</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/wurth-elektronik/61300611821/connector-rcpt-6pos-1row-2-54mm/dp/2827893</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,30 +886,30 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <f>SUM(I7:I43)</f>
-        <v>501.2940000000001</v>
+        <v>496.34400000000005</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <f>SUM(J7:J44)</f>
-        <v>449.36790000000013</v>
+        <v>448.87290000000013</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1008,7 +1008,7 @@
         <f t="shared" ref="J8:J15" si="0">G8*D8</f>
         <v>10.5</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1076,7 +1076,7 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
         <f t="shared" si="0"/>
         <v>35.9</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
         <f t="shared" si="0"/>
         <v>23.95</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
         <f t="shared" si="0"/>
         <v>14.9</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -1274,7 +1274,7 @@
       <c r="J16">
         <v>50</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
       <c r="J17">
         <v>50</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       <c r="J18">
         <v>200</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
         <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1468,7 +1468,7 @@
         <f t="shared" si="4"/>
         <v>0.14699999999999999</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
         <f t="shared" si="4"/>
         <v>0.72</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1536,16 +1536,16 @@
         <f t="shared" si="4"/>
         <v>0.24399999999999999</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" t="s">
         <v>142</v>
-      </c>
-      <c r="C27" t="s">
-        <v>143</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -1570,8 +1570,8 @@
         <f t="shared" si="4"/>
         <v>0.72199999999999998</v>
       </c>
-      <c r="K27" t="s">
-        <v>144</v>
+      <c r="K27" s="9" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1656,7 +1656,7 @@
         <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1682,7 +1682,7 @@
         <v>1.4419999999999999</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1789,16 +1789,16 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
         <v>109</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>110</v>
       </c>
       <c r="F36" s="3">
         <v>10707</v>
@@ -1819,7 +1819,7 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="K36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="25" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
         <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1841,25 +1841,25 @@
       <c r="E39" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="3">
-        <v>1109731</v>
+      <c r="F39" s="6">
+        <v>61300611821</v>
       </c>
       <c r="G39">
-        <v>0.78500000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H39">
         <v>10</v>
       </c>
       <c r="I39">
         <f t="shared" ref="I39:I40" si="11">H39*G39</f>
-        <v>7.8500000000000005</v>
+        <v>2.9</v>
       </c>
       <c r="J39">
         <f t="shared" ref="J39" si="12">G39*D39</f>
-        <v>0.78500000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K39" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1909,7 +1909,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>71</v>
@@ -1946,7 +1946,7 @@
         <v>65</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -1972,15 +1972,15 @@
         <v>0.442</v>
       </c>
       <c r="K44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -2006,7 +2006,7 @@
         <v>0.1694</v>
       </c>
       <c r="K45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2045,10 +2045,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2074,12 +2074,12 @@
         <v>1.3959999999999999</v>
       </c>
       <c r="K47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" s="5"/>
     </row>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51" t="s">
         <v>63</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
         <v>60</v>
@@ -2191,15 +2191,15 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" t="s">
         <v>117</v>
-      </c>
-      <c r="C55" t="s">
-        <v>118</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2208,7 +2208,7 @@
         <v>12</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G55">
         <v>1.5</v>
@@ -2225,15 +2225,15 @@
         <v>1.5</v>
       </c>
       <c r="K55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D56">
         <v>4</v>
@@ -2242,7 +2242,7 @@
         <v>34</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G56">
         <f>3.5/H56</f>
@@ -2260,21 +2260,21 @@
         <v>2.8</v>
       </c>
       <c r="K56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D57" s="12">
         <v>1</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F57" s="3">
         <v>11234</v>
@@ -2294,16 +2294,16 @@
         <v>6</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L57" s="12"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2329,15 +2329,15 @@
         <v>2.5</v>
       </c>
       <c r="K58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -2363,21 +2363,21 @@
         <v>7.5</v>
       </c>
       <c r="K59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C60" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
         <v>139</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>140</v>
       </c>
       <c r="F60" s="3">
         <v>1296899</v>
@@ -2398,7 +2398,7 @@
         <v>0.38</v>
       </c>
       <c r="K60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2409,6 +2409,21 @@
     <hyperlink ref="K7" r:id="rId1"/>
     <hyperlink ref="K14" r:id="rId2"/>
     <hyperlink ref="K57" r:id="rId3"/>
+    <hyperlink ref="K8" r:id="rId4"/>
+    <hyperlink ref="K9" r:id="rId5"/>
+    <hyperlink ref="K10" r:id="rId6"/>
+    <hyperlink ref="K11" r:id="rId7"/>
+    <hyperlink ref="K12" r:id="rId8"/>
+    <hyperlink ref="K13" r:id="rId9"/>
+    <hyperlink ref="K15" r:id="rId10"/>
+    <hyperlink ref="K16" r:id="rId11"/>
+    <hyperlink ref="K17" r:id="rId12"/>
+    <hyperlink ref="K18" r:id="rId13"/>
+    <hyperlink ref="K23" r:id="rId14"/>
+    <hyperlink ref="K24" r:id="rId15"/>
+    <hyperlink ref="K25" r:id="rId16"/>
+    <hyperlink ref="K26" r:id="rId17"/>
+    <hyperlink ref="K27" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>